<commit_message>
Update Buat SImulasi Kredit
</commit_message>
<xml_diff>
--- a/EditEmaildanNomor.xlsx
+++ b/EditEmaildanNomor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\magangg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\magangg\ACC-ACCPartner\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="20">
   <si>
     <t>username</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Terverifikasi</t>
+  </si>
+  <si>
+    <t>Belum Terverifikasi</t>
   </si>
 </sst>
 </file>
@@ -410,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,14 +568,68 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="D4" r:id="rId3"/>
     <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>